<commit_message>
updating test case scenarios
</commit_message>
<xml_diff>
--- a/Test_Cases_&_Scenarios/CourseL-AI.xlsx
+++ b/Test_Cases_&_Scenarios/CourseL-AI.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CourseL-AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CourseL-AI\Test_Cases_&amp;_Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Platform" sheetId="1" r:id="rId1"/>
     <sheet name="Features_Front&amp;Backend" sheetId="4" r:id="rId2"/>
     <sheet name="Frontend_Functionalities" sheetId="6" r:id="rId3"/>
     <sheet name="Backend_Functionalities" sheetId="5" r:id="rId4"/>
+    <sheet name="TS_FrontEnd" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>Website</t>
   </si>
@@ -172,13 +173,165 @@
   </si>
   <si>
     <t>Users can Perform login with Gmail</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Users can see the profile details</t>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>Users can get subscription plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings </t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>Users can sign out</t>
+  </si>
+  <si>
+    <t>Users can manage account settings</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>Users can see &amp; start any program</t>
+  </si>
+  <si>
+    <t>User can see &amp; complete any courses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can get the cerificates of the courses </t>
+  </si>
+  <si>
+    <t>Test case title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case scenario </t>
+  </si>
+  <si>
+    <t>Verify that nevigation bar showes at the top after laods.</t>
+  </si>
+  <si>
+    <t>Verify that logo is visiable in the nagivation</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on logo redirect users to the home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Home" button is clickable or not </t>
+  </si>
+  <si>
+    <t>Verify that after loads "Courses" button is visiable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Courses" button is clickable or not </t>
+  </si>
+  <si>
+    <t>Verify that after loads "Pricing" button is visiable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Pricing" button is clickable or not </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that after loads "Support" option is visiable </t>
+  </si>
+  <si>
+    <t>Verify that sub menu items are appear when hovering over the "Support"</t>
+  </si>
+  <si>
+    <t>Verify that top navigation bar is consistent across all pages</t>
+  </si>
+  <si>
+    <t>Verify that "Login" / "Join Now" buttons appear only when logged out</t>
+  </si>
+  <si>
+    <t>Verify that sub menu items of "Support" are clickable or not</t>
+  </si>
+  <si>
+    <t>Verify that "Enroll Free" button is visiable or not</t>
+  </si>
+  <si>
+    <t>Verify that "Enroll Free" button is clickable or not</t>
+  </si>
+  <si>
+    <t>Verify that "Start Now" button is visiable or not</t>
+  </si>
+  <si>
+    <t>Verify that "Start Your Journey" button is visiable or not</t>
+  </si>
+  <si>
+    <t>Verify that "Start Your Journey" button is clickable or not</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on "Enroll Free" button redirect users to the "Pricing" page</t>
+  </si>
+  <si>
+    <t>Verify that "Start Now" button is clickable or not</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on "Start Now" button redirect users to the "Pricing" page</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on "Start Your Journey" button redirect users to the "Pricing" page</t>
+  </si>
+  <si>
+    <t>Verify that a promotional video is visiable in the Home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that promotional video is playing successfully </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Users can see the comments from previous students</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that students remarks are visiable in the home page</t>
+  </si>
+  <si>
+    <t>Verify that comments from the students are moving</t>
+  </si>
+  <si>
+    <t>Verify that users can see the questions &amp; answers in the FAQ section in the home page.</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on "+" button questions are opening with the answer.</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on "-" button answer are minimized</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,11 +373,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF09090B"/>
-      <name val="Outfit"/>
     </font>
     <font>
       <sz val="10"/>
@@ -279,6 +427,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -318,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -424,17 +578,6 @@
       <right style="thin">
         <color theme="4" tint="-0.249977111117893"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="4" tint="-0.249977111117893"/>
-      </right>
       <top style="thin">
         <color theme="4" tint="-0.249977111117893"/>
       </top>
@@ -456,40 +599,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="2"/>
+      </left>
+      <right style="medium">
+        <color theme="2"/>
+      </right>
+      <top style="medium">
+        <color theme="2"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA4C2F4"/>
+      </right>
+      <top style="medium">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA4C2F4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA4C2F4"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFA4C2F4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA4C2F4"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA4C2F4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="2"/>
+      </left>
+      <right style="medium">
+        <color theme="2"/>
+      </right>
+      <top style="medium">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -500,35 +778,58 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,33 +1052,33 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -803,128 +1104,128 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A1" s="22" t="str">
+    <row r="1" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="str">
         <f>HYPERLINK("https://coursel.app/", "Frontend")</f>
         <v>Frontend</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:2" ht="27" customHeight="1" thickBot="1">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:2" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" customHeight="1">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" customHeight="1">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" customHeight="1">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A8" s="22" t="str">
+    <row r="8" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="str">
         <f>HYPERLINK("https://learning.coursel.app/mastery","Backend")</f>
         <v>Backend</v>
       </c>
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="1:2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A9" s="24" t="s">
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18" customHeight="1" thickBot="1">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="8" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:2" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" customHeight="1" thickBot="1">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" customHeight="1">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18" customHeight="1" thickBot="1">
-      <c r="A14" s="21" t="s">
+    <row r="14" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -949,152 +1250,152 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="43" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="12.5703125" style="8"/>
+    <col min="1" max="1" width="24.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="43" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="12.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" customHeight="1">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25"/>
+      <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" customHeight="1">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1115,228 +1416,487 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.75">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75">
-      <c r="A3" s="14"/>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.75">
-      <c r="A4" s="14"/>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21"/>
+      <c r="B4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75">
-      <c r="A5" s="15"/>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.75">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="12.75">
-      <c r="A7" s="14"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="12.75">
-      <c r="A8" s="14"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="12.75">
-      <c r="A9" s="14"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="12.75">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="12.75">
-      <c r="A11" s="14"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="12.75">
-      <c r="A12" s="14"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="12.75">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="12.75">
-      <c r="A14" s="14"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="12.75">
-      <c r="A15" s="14"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="12.75">
-      <c r="A16" s="14"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="12.75">
-      <c r="A18" s="14"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="17"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="17"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="18" t="s">
+      <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="19"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="12" t="s">
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="12"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="12.5703125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="42"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B2:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updating frontEnd test scenarios
</commit_message>
<xml_diff>
--- a/Test_Cases_&_Scenarios/CourseL-AI.xlsx
+++ b/Test_Cases_&_Scenarios/CourseL-AI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Platform" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Frontend_Functionalities" sheetId="6" r:id="rId3"/>
     <sheet name="Backend_Functionalities" sheetId="5" r:id="rId4"/>
     <sheet name="TS_FrontEnd" sheetId="7" r:id="rId5"/>
+    <sheet name="TS_BackEnd" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
   <si>
     <t>Website</t>
   </si>
@@ -325,6 +326,72 @@
   </si>
   <si>
     <t>Verify that after clicking on "-" button answer are minimized</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Verify that various courses cart is showing in Courses page.</t>
+  </si>
+  <si>
+    <t>Verify that courses details are displayed correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that after clicking on any course cart the course details are opening into new page </t>
+  </si>
+  <si>
+    <t>Verify that paid &amp; bonus courses are showing at the top</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on the paid or bonus courses the course details are opening into new page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "&lt;" &amp; "&gt;" buttons are working or not </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that filter option is showing or not </t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Short By : " dropdown is opening</t>
+  </si>
+  <si>
+    <t>Verify that "Short By: " sub menus are working or not</t>
+  </si>
+  <si>
+    <t>Verify that after changing the sub menu option of filter , values are also change in "Short By : " accordingly</t>
+  </si>
+  <si>
+    <t>Verify that price based filter optiuon is visiable or not</t>
+  </si>
+  <si>
+    <t>Verify that price based filter options are working &amp; changing data accordingly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "clear all" button is working or not </t>
+  </si>
+  <si>
+    <t>Verify that "Pick Your Plan, Master AI Fast" title is showing on the top of Pricing page</t>
+  </si>
+  <si>
+    <t>Verify that enrollment cart is showing or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that prices are showing correctly or not </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that "Get Now" button is working or not </t>
+  </si>
+  <si>
+    <t>Verify that "Contact with Email" is showing in sub menu</t>
+  </si>
+  <si>
+    <t>Verify that "Contact with Email" is working or not</t>
+  </si>
+  <si>
+    <t>Verify that "Contact with WhatsApp" is showing in sub menu</t>
+  </si>
+  <si>
+    <t>Verify that "Contact with WhatsApp" is working or not</t>
   </si>
 </sst>
 </file>
@@ -434,7 +501,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +536,18 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -724,7 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,6 +834,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -781,55 +873,65 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1059,25 +1161,25 @@
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1114,11 +1216,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="str">
+      <c r="A1" s="23" t="str">
         <f>HYPERLINK("https://coursel.app/", "Frontend")</f>
         <v>Frontend</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:2" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -1129,51 +1231,51 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="str">
+      <c r="A8" s="23" t="str">
         <f>HYPERLINK("https://learning.coursel.app/mastery","Backend")</f>
         <v>Backend</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1184,42 +1286,42 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1250,7 +1352,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1273,7 +1375,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -1284,7 +1386,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1293,7 +1395,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1302,7 +1404,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1311,7 +1413,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1322,7 +1424,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1331,7 +1433,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1340,7 +1442,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1349,7 +1451,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1360,7 +1462,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
@@ -1380,7 +1482,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1391,7 +1493,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
@@ -1418,8 +1520,8 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1430,18 +1532,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -1452,7 +1554,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1461,7 +1563,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="1" t="s">
         <v>44</v>
       </c>
@@ -1470,7 +1572,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1479,7 +1581,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1490,7 +1592,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
@@ -1499,7 +1601,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
@@ -1508,7 +1610,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="1" t="s">
         <v>55</v>
       </c>
@@ -1564,10 +1666,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1579,21 +1681,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="38" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -1601,50 +1703,50 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1652,15 +1754,15 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="38"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="39" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1668,15 +1770,15 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1684,17 +1786,17 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="38"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1702,64 +1804,64 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="37"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="37"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="38"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="39" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1767,15 +1869,15 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="38"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="36" t="s">
         <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1783,15 +1885,15 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="39" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1799,91 +1901,194 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="37"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="38"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="A31" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="A44" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="42"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="42"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="50"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="43"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="43"/>
+      <c r="B50" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="48"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A44:A47"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="A15:A30"/>
     <mergeCell ref="B13:B14"/>
@@ -1891,14 +2096,315 @@
     <mergeCell ref="B15:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B2:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="14" customWidth="1"/>
+    <col min="4" max="16384" width="12.5703125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="46"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="35"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="43"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="43"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="43"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="43"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="43"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="48"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="49"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="42"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="42"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="50"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="47"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="43"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="43"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="48"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update backEnd test case scenarios
</commit_message>
<xml_diff>
--- a/Test_Cases_&_Scenarios/CourseL-AI.xlsx
+++ b/Test_Cases_&_Scenarios/CourseL-AI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Platform" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="151">
   <si>
     <t>Website</t>
   </si>
@@ -392,6 +392,111 @@
   </si>
   <si>
     <t>Verify that "Contact with WhatsApp" is working or not</t>
+  </si>
+  <si>
+    <t>Verify that " Login " button is showing on navigation bar</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Login " button it redirect the users to login form page</t>
+  </si>
+  <si>
+    <t>Verify that " Email address " &amp; " Password " field is available on login form</t>
+  </si>
+  <si>
+    <t>Verify that " Log In " button is available on login form</t>
+  </si>
+  <si>
+    <t>Verify that " Log In To Coursel " headline is showing on the top of login form</t>
+  </si>
+  <si>
+    <t>Verify that users can login with the already registered data</t>
+  </si>
+  <si>
+    <t>Vefiry that users can't login without registered data</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Forget Password? " it redirect the users to " Forgot Password " page</t>
+  </si>
+  <si>
+    <t>Verify that users can send their registered mail for reset password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for reset password user can use unregistered any email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that after sending email for passowrd reset " Mail Sent! " confirmation message is showing </t>
+  </si>
+  <si>
+    <t>Verify that " Enter Your Email address " is visiable in " Email Address " field</t>
+  </si>
+  <si>
+    <t>Verify that " Enter Your Password " is visiable in " Password " field</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Join Now" button it redirect the users to the Sign up page</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Sign up" button in " Log in " page it redirect the users to the Sign up page</t>
+  </si>
+  <si>
+    <t>Verify that " Sign Up To Coursel " headline is showing at the top</t>
+  </si>
+  <si>
+    <t>Register with Gmail</t>
+  </si>
+  <si>
+    <t>Users can register with Gmail</t>
+  </si>
+  <si>
+    <t>Verify that users can register with valid information</t>
+  </si>
+  <si>
+    <t>Verify that users can register with missing required information</t>
+  </si>
+  <si>
+    <t>Verify that user can register using existing email</t>
+  </si>
+  <si>
+    <t>Verify that users can use only numeric number as name for " Name " field</t>
+  </si>
+  <si>
+    <t>Verify that users can use alphanumeric data as name for " Name " field</t>
+  </si>
+  <si>
+    <t>Verify that use can take unvalid email</t>
+  </si>
+  <si>
+    <t>Verify that after missing information in " Name " filed " Name must be at least 2 characters" is showing</t>
+  </si>
+  <si>
+    <t>Verify that after missing information in " Email address " field " Please enter a valid email address "  is showing</t>
+  </si>
+  <si>
+    <t>Verify that users can take less than 8 charecters for password</t>
+  </si>
+  <si>
+    <t>Verify that hide password button in the " Password " &amp; "Confirm Password" field is working</t>
+  </si>
+  <si>
+    <t>Verify that hide password button in the " Password " field is working</t>
+  </si>
+  <si>
+    <t>Verify that " Forget Password? " button is available on Log in form</t>
+  </si>
+  <si>
+    <t>Verify that " Sign in with Gmail" button is available in login form</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Sign in with Gmail" button it redirect the users to gmail login page</t>
+  </si>
+  <si>
+    <t>Verify that after adding any email it redirect the users to the users dashboard</t>
+  </si>
+  <si>
+    <t>Verify that " Continue with Gmail" button is available in sign up form</t>
+  </si>
+  <si>
+    <t>Verify that after clicking on " Continue with Gmail" button it redirect the users to gmail login page</t>
   </si>
 </sst>
 </file>
@@ -501,7 +606,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,8 +655,14 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -798,12 +909,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA4C2F4"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA4C2F4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFA4C2F4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39991454817346722"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA4C2F4"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA4C2F4"/>
+      </right>
+      <top style="medium">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39988402966399123"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39988402966399123"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39988402966399123"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39988402966399123"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39988402966399123"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -847,6 +1054,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,21 +1081,57 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -897,40 +1141,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1155,31 +1414,31 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="22"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1216,11 +1475,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="str">
+      <c r="A1" s="24" t="str">
         <f>HYPERLINK("https://coursel.app/", "Frontend")</f>
         <v>Frontend</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -1271,11 +1530,11 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="str">
+      <c r="A8" s="24" t="str">
         <f>HYPERLINK("https://learning.coursel.app/mastery","Backend")</f>
         <v>Backend</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="25"/>
     </row>
     <row r="9" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1375,7 +1634,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -1386,7 +1645,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1395,7 +1654,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1404,7 +1663,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1413,7 +1672,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1424,7 +1683,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1433,7 +1692,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1442,7 +1701,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1451,7 +1710,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1462,7 +1721,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
@@ -1482,7 +1741,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1493,7 +1752,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
@@ -1518,10 +1777,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1543,7 +1802,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -1562,7 +1821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
       <c r="B4" s="1" t="s">
         <v>44</v>
@@ -1571,8 +1830,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
       <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1580,81 +1839,90 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:3" s="19" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1668,8 +1936,8 @@
   </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1692,10 +1960,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="51" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -1703,50 +1971,50 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="31" t="s">
+      <c r="A9" s="47"/>
+      <c r="B9" s="37" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1754,15 +2022,15 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="37" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1770,15 +2038,15 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="37" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1786,17 +2054,17 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1804,64 +2072,64 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="32"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="32"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="37" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1869,15 +2137,15 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36" t="s">
+      <c r="A26" s="45"/>
+      <c r="B26" s="49" t="s">
         <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1885,15 +2153,15 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="37"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="45"/>
+      <c r="B28" s="37" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1901,24 +2169,24 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="32"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1926,43 +2194,43 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="41"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="39" t="s">
+      <c r="A37" s="35"/>
+      <c r="B37" s="32" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1970,52 +2238,52 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="40"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="32" t="s">
         <v>38</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -2023,31 +2291,31 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="41"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="32" t="s">
         <v>40</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -2055,15 +2323,15 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="41"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="33"/>
       <c r="C49" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="39" t="s">
+      <c r="A50" s="35"/>
+      <c r="B50" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2071,14 +2339,16 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="48"/>
-      <c r="B51" s="41"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="33"/>
       <c r="C51" s="1" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B2:B8"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="A48:A51"/>
@@ -2095,8 +2365,6 @@
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="B15:B23"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B2:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2108,10 +2376,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2126,7 +2394,7 @@
       <c r="A1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -2134,275 +2402,513 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="53" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="53" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="53" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="53" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="53" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="53" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="53" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="53" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="53" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="53" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="53" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="53" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="53" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="65"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="53" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="65"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="53" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="53" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="53" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="53" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="53" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="53" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="53" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="65"/>
+      <c r="B25" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="53" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="53" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="1"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="53" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="65"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="53" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="1"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="39"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="1"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="1"/>
+      <c r="A35" s="65"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="41"/>
+      <c r="A36" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="60"/>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="61"/>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="32"/>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="40"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="59"/>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="61"/>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="41"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="61"/>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
-      <c r="B48" s="39"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="61"/>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="41"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="61"/>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="39"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="61"/>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="48"/>
-      <c r="B51" s="41"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="61"/>
       <c r="C51" s="1"/>
     </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="35"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="35"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="36"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="34"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="35"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="35"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="36"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="35"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="36"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="34"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="35"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="35"/>
+      <c r="B65" s="61"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="36"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="34"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="35"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="35"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="36"/>
+      <c r="B70" s="61"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="34"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="35"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="35"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="36"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="34"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="35"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="35"/>
+      <c r="B77" s="61"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="36"/>
+      <c r="B78" s="61"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="34"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="35"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="36"/>
+      <c r="B82" s="61"/>
+      <c r="C82" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A31:A43"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A30"/>
-    <mergeCell ref="B15:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B30"/>
+  <mergeCells count="19">
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="B12:B24"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A2:A35"/>
+    <mergeCell ref="A36:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>